<commit_message>
new preparation file versuch 7.csv
</commit_message>
<xml_diff>
--- a/scrapers/TA/scrapes/WEKA/Sci-Kit Preparation/data/Versuch_6.xlsx
+++ b/scrapers/TA/scrapes/WEKA/Sci-Kit Preparation/data/Versuch_6.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TobiasRordorf/Desktop/UNI/MBI HSG/4. Semester/Python/GitHub/hotelierchallenge/scrapers/TA/scrapes/WEKA/Sci-Kit Preparation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CA3FB4-B531-6045-A8FB-F6A298B6CB12}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A02974-7A31-0240-8EAB-C08F06E0C3C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6660" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Versuch_5" sheetId="1" r:id="rId1"/>
+    <sheet name="Versuch_6" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -498,8 +498,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -855,46 +856,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K386"/>
+  <dimension ref="A1:K377"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C390" sqref="C390:D390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
         <v>2</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>3</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>4</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>5</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="1">
         <v>6</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="1">
         <v>7</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="1">
         <v>8</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="1">
         <v>9</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="1">
         <v>10</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="1">
         <v>11</v>
       </c>
     </row>
@@ -14055,186 +14056,6 @@
         <v>1.103</v>
       </c>
       <c r="K377">
-        <v>1.0289999999999999</v>
-      </c>
-    </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A378">
-        <v>0.94</v>
-      </c>
-      <c r="B378">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="C378">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="D378">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="E378">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="F378">
-        <v>0.98</v>
-      </c>
-      <c r="G378">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="H378">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="I378">
-        <v>1.103</v>
-      </c>
-      <c r="J378">
-        <v>1.0289999999999999</v>
-      </c>
-    </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A379">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="B379">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="C379">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="D379">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="E379">
-        <v>0.98</v>
-      </c>
-      <c r="F379">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="G379">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="H379">
-        <v>1.103</v>
-      </c>
-      <c r="I379">
-        <v>1.0289999999999999</v>
-      </c>
-    </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A380">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="B380">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="C380">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="D380">
-        <v>0.98</v>
-      </c>
-      <c r="E380">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="F380">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="G380">
-        <v>1.103</v>
-      </c>
-      <c r="H380">
-        <v>1.0289999999999999</v>
-      </c>
-    </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A381">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="B381">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="C381">
-        <v>0.98</v>
-      </c>
-      <c r="D381">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="E381">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="F381">
-        <v>1.103</v>
-      </c>
-      <c r="G381">
-        <v>1.0289999999999999</v>
-      </c>
-    </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A382">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="B382">
-        <v>0.98</v>
-      </c>
-      <c r="C382">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="D382">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="E382">
-        <v>1.103</v>
-      </c>
-      <c r="F382">
-        <v>1.0289999999999999</v>
-      </c>
-    </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A383">
-        <v>0.98</v>
-      </c>
-      <c r="B383">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="C383">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="D383">
-        <v>1.103</v>
-      </c>
-      <c r="E383">
-        <v>1.0289999999999999</v>
-      </c>
-    </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A384">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="B384">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="C384">
-        <v>1.103</v>
-      </c>
-      <c r="D384">
-        <v>1.0289999999999999</v>
-      </c>
-    </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A385">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="B385">
-        <v>1.103</v>
-      </c>
-      <c r="C385">
-        <v>1.0289999999999999</v>
-      </c>
-    </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A386">
-        <v>1.103</v>
-      </c>
-      <c r="B386">
         <v>1.0289999999999999</v>
       </c>
     </row>

</xml_diff>